<commit_message>
Made some preliminary plots for revisions
</commit_message>
<xml_diff>
--- a/Supplemental_tables/Table S1.xlsx
+++ b/Supplemental_tables/Table S1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28605"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/embree_14_buckeyemail_osu_edu/Documents/Splicing and NMD/Final_Manuscript/Supplemental_Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{8609F455-67A5-44B2-BAF7-8F8D5EB88440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA41861D-7E6D-4CC5-A05D-A9BA50B45FCF}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{8609F455-67A5-44B2-BAF7-8F8D5EB88440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325D87E7-DE64-4B10-92C3-C4675CCF179E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDD03918-7167-4DA3-8D5C-F77FDB368A79}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" xr2:uid="{CDD03918-7167-4DA3-8D5C-F77FDB368A79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -39,12 +39,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="185">
   <si>
     <t>Accesion numbers of all datasets used in this study.</t>
   </si>
   <si>
-    <t>Separated by the type of data: depletion of spliceosome componenets from ENCODE, treatment with splice altering drugs, and cells with spliceosome mutations.</t>
+    <t>Separated by the type of data: depletion of spliceosome componenets from ENCODE,</t>
+  </si>
+  <si>
+    <t>treatment with splice altering drugs, and cells with spliceosome mutations.</t>
   </si>
   <si>
     <t xml:space="preserve">DOI to the publications from the later two groups are also included. </t>
@@ -503,7 +506,7 @@
     <t>SRR24900084</t>
   </si>
   <si>
-    <t>Risdiplam</t>
+    <t>Risdiplam*</t>
   </si>
   <si>
     <t>lymphoblastoid cells</t>
@@ -527,7 +530,7 @@
     <t>doi:10.1038/s41588-024-01872-x</t>
   </si>
   <si>
-    <t>note: The runs in each box were merged to form one replicate</t>
+    <t>*note: The runs in each box were merged to form one replicate</t>
   </si>
   <si>
     <t>Spliceosome Component</t>
@@ -597,7 +600,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +639,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -663,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -677,6 +686,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,9 +1021,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008C7078-76BB-4441-BCF7-166900F9C243}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1030,793 +1040,819 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CBD621-C2A0-41BB-BE70-F006D511DF19}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
     <sortCondition ref="A2:A22"/>
   </sortState>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A964E2-09ED-434A-A0E9-4F8D970D6365}">
-  <dimension ref="A1:J5"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="7" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="5" t="s">
+      <c r="F3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>140</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="J5" s="6" t="s">
         <v>162</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069F333E-7DF4-4036-A2E5-1DC6B6776DF5}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1833,92 +1869,94 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>